<commit_message>
Alpha version Input & CARGO update
</commit_message>
<xml_diff>
--- a/data/input_mail/mail_copy_in_format_22_08.xlsx
+++ b/data/input_mail/mail_copy_in_format_22_08.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="27750" windowHeight="11770" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="27750" windowHeight="11770" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ELMONGY" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="469">
   <si>
     <t>SHIPPER NAME :</t>
   </si>
@@ -3830,7 +3830,7 @@
   <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4440,10 +4440,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4609,96 +4609,71 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>